<commit_message>
Implement API client for inventory management, including CRUD operations for products, suppliers, and locations. Introduce data migration utilities for transferring existing Excel data to the new API structure. Enhance the Streamlit app to support API interactions with fallback to Excel. Update documentation for migration and API usage.
</commit_message>
<xml_diff>
--- a/data/fournisseurs.xlsx
+++ b/data/fournisseurs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,17 +471,17 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>Nb_Produits</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Valeur_Stock_Total</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>Date_Creation</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Nb_Produits</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Valeur_Stock_Total</t>
         </is>
       </c>
     </row>
@@ -493,7 +493,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BOSCHAT</t>
+          <t>Fournisseur C</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -503,134 +503,26 @@
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>À définir</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
           <t>Actif</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>2025-05-26</t>
-        </is>
+      <c r="H2" t="n">
+        <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>13</v>
-      </c>
-      <c r="J2" t="n">
-        <v>4208.36</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>FOUR002</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>FAILLE</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>À définir</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Actif</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>2025-05-26</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
-        <v>2</v>
-      </c>
-      <c r="J3" t="n">
-        <v>192.37</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>FOUR003</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>SFS</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>À définir</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Actif</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>2025-05-26</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
-        <v>2</v>
-      </c>
-      <c r="J4" t="n">
-        <v>6923.18</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>FOUR004</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>FournX</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>À définir</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>À définir</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Actif</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>2025-05-28</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" t="n">
-        <v>1125</v>
+        <v>0</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>